<commit_message>
bug fixed for rounding
</commit_message>
<xml_diff>
--- a/scoring/forms/EMSS/EMSS47_test_1.xlsx
+++ b/scoring/forms/EMSS/EMSS47_test_1.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="question_answers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="outputs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -906,4 +907,265 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>پاسخ سیستم</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>پاسخ دستی کارشناس</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>raw</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>t_score</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>t_score_summary</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>عدم رضایت از روابط زناشویی همسران</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>marital_communication</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>personality_issues</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>religious_orientation</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Conflict_resolution</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>financial_management</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>leisure_activities</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>sexual_relationship</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>children_&amp;_marriage</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>family_&amp;_friends</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>personality_issues_interpretation</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>رضایت زیاد</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>marital_communication_interpretation</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>رضایت متوسط</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Conflict_resolution_interpretation</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>رضایت متوسط</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>financial_management_interpretation</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>رضایت متوسط</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>leisure_activities_interpretation</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>رضایت متوسط</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>sexual_relationship_interpretation</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>رضایت متوسط</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>children_&amp;_marriage_interpretation</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>رضایت متوسط</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>family_&amp;_friends_interpretation</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>عدم رضایت</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>religious_orientation_interpretation</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>رضایت متوسط</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>